<commit_message>
retry to commit repository
</commit_message>
<xml_diff>
--- a/corona-cases-kuwait.xlsx
+++ b/corona-cases-kuwait.xlsx
@@ -1489,6 +1489,17 @@
           </cell>
           <cell r="J128">
             <v>8861</v>
+          </cell>
+        </row>
+        <row r="129">
+          <cell r="B129">
+            <v>44012</v>
+          </cell>
+          <cell r="C129">
+            <v>671</v>
+          </cell>
+          <cell r="J129">
+            <v>8811</v>
           </cell>
         </row>
       </sheetData>
@@ -1786,10 +1797,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C128"/>
+  <dimension ref="A1:C129"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView tabSelected="1" topLeftCell="A106" workbookViewId="0">
+      <selection activeCell="A130" sqref="A130"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3585,6 +3596,20 @@
       <c r="C128">
         <f>[1]Sheet2!J128</f>
         <v>8861</v>
+      </c>
+    </row>
+    <row r="129" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A129" s="1">
+        <f>[1]Sheet2!B129</f>
+        <v>44012</v>
+      </c>
+      <c r="B129">
+        <f>[1]Sheet2!C129</f>
+        <v>671</v>
+      </c>
+      <c r="C129">
+        <f>[1]Sheet2!J129</f>
+        <v>8811</v>
       </c>
     </row>
   </sheetData>

</xml_diff>